<commit_message>
fixes to the test documents
</commit_message>
<xml_diff>
--- a/Docs/TestInvoice1.xlsx
+++ b/Docs/TestInvoice1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Template1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Bill To</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>DueDate</t>
   </si>
   <si>
     <t>Description</t>
@@ -197,9 +194,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -207,12 +201,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -225,6 +213,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -543,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,16 +551,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="A1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -572,85 +569,85 @@
       <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>15</v>
+      <c r="H3" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
       <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>16</v>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f ca="1">TODAY()</f>
         <v>42806</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="3">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2">
         <f ca="1">H5+30</f>
         <v>42836</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="7">
+      <c r="B10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="6">
         <v>150</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <f>G10*A10</f>
         <v>150</v>
       </c>
@@ -659,17 +656,17 @@
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="7">
+      <c r="B11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="6">
         <v>87.56</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <f t="shared" ref="H11:H12" si="0">G11*A11</f>
         <v>437.8</v>
       </c>
@@ -678,44 +675,44 @@
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="7">
+      <c r="B12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="6">
         <v>36.5</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <f t="shared" si="0"/>
         <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="11">
+        <v>11</v>
+      </c>
+      <c r="H14" s="8">
         <f>SUM(H10:H12)</f>
         <v>879.8</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="11">
+        <v>12</v>
+      </c>
+      <c r="H15" s="8">
         <f>H14*0.13</f>
         <v>114.374</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="G16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="6">
+      <c r="G16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="5">
         <f>H15+H14</f>
         <v>994.17399999999998</v>
       </c>
@@ -739,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -755,100 +752,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="A1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="15">
+      <c r="E4" s="12">
         <f ca="1">TODAY()</f>
         <v>42806</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="12">
         <f ca="1">E4+30</f>
         <v>42836</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="H6" s="3"/>
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="7">
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="6">
         <v>150</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f>E10*A10</f>
         <v>150</v>
       </c>
@@ -857,15 +854,15 @@
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7">
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6">
         <v>87.56</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f>E11*A11</f>
         <v>437.8</v>
       </c>
@@ -874,42 +871,42 @@
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="7">
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6">
         <v>36.5</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f>E12*A12</f>
         <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="11">
+        <v>11</v>
+      </c>
+      <c r="F14" s="8">
         <f>SUM(F10:F12)</f>
         <v>879.8</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="11">
+        <v>12</v>
+      </c>
+      <c r="F15" s="8">
         <f>F14*0.13</f>
         <v>114.374</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="E16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5">
         <f>F15+F14</f>
         <v>994.17399999999998</v>
       </c>

</xml_diff>